<commit_message>
Major Update: - Changed Request Method for Type GET, from Array to Object - Many fixbug
</commit_message>
<xml_diff>
--- a/manual for dev.xlsx
+++ b/manual for dev.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
-  <si>
-    <t>FAQ / Description</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Location</t>
   </si>
@@ -31,9 +28,6 @@
   </si>
   <si>
     <t>Type</t>
-  </si>
-  <si>
-    <t>Example</t>
   </si>
   <si>
     <t>Filter Record</t>
@@ -128,11 +122,61 @@
   <si>
     <t>Sort/Order</t>
   </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>What inside models.php</t>
+  </si>
+  <si>
+    <t>What inside controller.php</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>FAQ</t>
+  </si>
+  <si>
+    <t>What Request Method for?</t>
+  </si>
+  <si>
+    <t>UNLOCK &amp; LOCK = for login &amp; unlock screen
+PATCH = for selection role window
+GET = for view
+POST = for insert
+PUT = for update
+DELETE = for delete
+OPTIONS = for reporting</t>
+  </si>
+  <si>
+    <t>Request Method Event</t>
+  </si>
+  <si>
+    <t>UNLOCK &amp; LOCK = no event
+PATCH = no event
+GET = pre_get
+POST &amp; PUT = pre_post_put, pre_post, pre_put, post_post_put, post_post, post_put
+DELETE = pre_delete, post_delete
+OPTIONS = pre_options</t>
+  </si>
+  <si>
+    <t>function name same as name file &amp; function name in controller
+Ex: 
+- view filename = cf_sorder.tpl
+- method/function = cf_sorder()</t>
+  </si>
+  <si>
+    <t>function name same as name file &amp; function name in model
+Ex: 
+- view filename = cf_sorder.tpl
+- method/function = cf_sorder()</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -461,67 +505,106 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="18.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.5703125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="18.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="189" style="1" customWidth="1"/>
+    <col min="5" max="5" width="130.7109375" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>